<commit_message>
test jurisdiction update and test bug fix
</commit_message>
<xml_diff>
--- a/test_codecept/e2e/documents/ccd-config-aat-xui-testCaseType_v2.dev.xlsx
+++ b/test_codecept/e2e/documents/ccd-config-aat-xui-testCaseType_v2.dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreekanth/work/moj/ex-ui/ccd_def/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreekanth/work/moj/ex-ui/rpx-xui-webapp/test_codecept/e2e/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D4D39C-E1D7-4344-94A4-08521F2DBC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDA13CF9-2A06-2946-9523-6111C0648949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33480" windowHeight="18600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33480" windowHeight="18600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -6527,8 +6527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8622,8 +8622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9848,7 +9848,7 @@
         <v>27</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
functional e2e feature split and logs update
</commit_message>
<xml_diff>
--- a/test_codecept/e2e/documents/ccd-config-aat-xui-testCaseType_v2.dev.xlsx
+++ b/test_codecept/e2e/documents/ccd-config-aat-xui-testCaseType_v2.dev.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreekanth/work/moj/ex-ui/rpx-xui-webapp/test_codecept/e2e/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDA13CF9-2A06-2946-9523-6111C0648949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EA2230-70FB-0945-B9DC-5ABB01D06A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33480" windowHeight="18600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33480" windowHeight="18600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="386">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -6527,7 +6527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -8620,10 +8620,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9839,23 +9839,25 @@
         <v>384</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="E28" s="72" t="s">
-        <v>382</v>
+        <v>198</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="F28" s="21">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="I28" s="12"/>
+        <v>187</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>188</v>
+      </c>
       <c r="J28" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -9883,13 +9885,13 @@
         <v>198</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F29" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>187</v>
@@ -9901,18 +9903,18 @@
         <v>1</v>
       </c>
       <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
       <c r="N29" s="7"/>
       <c r="O29" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
-      <c r="U29" s="27"/>
+      <c r="U29" s="30"/>
     </row>
     <row r="30" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
@@ -9926,10 +9928,10 @@
         <v>198</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F30" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>190</v>
@@ -9948,14 +9950,13 @@
       <c r="M30" s="12"/>
       <c r="N30" s="7"/>
       <c r="O30" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
-      <c r="U30" s="30"/>
     </row>
     <row r="31" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
@@ -9969,10 +9970,10 @@
         <v>198</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F31" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>190</v>
@@ -9988,10 +9989,10 @@
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
+      <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
@@ -10011,10 +10012,10 @@
         <v>198</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F32" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>190</v>
@@ -10030,10 +10031,10 @@
       </c>
       <c r="K32" s="7"/>
       <c r="L32" s="12"/>
-      <c r="M32" s="7"/>
+      <c r="M32" s="12"/>
       <c r="N32" s="7"/>
       <c r="O32" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
@@ -10053,10 +10054,10 @@
         <v>198</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F33" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>190</v>
@@ -10075,7 +10076,7 @@
       <c r="M33" s="12"/>
       <c r="N33" s="7"/>
       <c r="O33" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
@@ -10095,29 +10096,29 @@
         <v>198</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F34" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>190</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="J34" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
       <c r="N34" s="7"/>
       <c r="O34" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
@@ -10137,10 +10138,10 @@
         <v>198</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F35" s="21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>190</v>
@@ -10159,7 +10160,7 @@
       <c r="M35" s="12"/>
       <c r="N35" s="7"/>
       <c r="O35" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
@@ -10179,10 +10180,10 @@
         <v>198</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F36" s="21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>190</v>
@@ -10201,7 +10202,7 @@
       <c r="M36" s="12"/>
       <c r="N36" s="7"/>
       <c r="O36" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
@@ -10221,10 +10222,10 @@
         <v>198</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F37" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>190</v>
@@ -10243,7 +10244,7 @@
       <c r="M37" s="12"/>
       <c r="N37" s="7"/>
       <c r="O37" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
@@ -10263,10 +10264,10 @@
         <v>198</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F38" s="21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>190</v>
@@ -10305,29 +10306,29 @@
         <v>198</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F39" s="21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G39" s="12" t="s">
         <v>190</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J39" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K39" s="7"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="7"/>
       <c r="O39" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
@@ -10347,13 +10348,13 @@
         <v>198</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F40" s="21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>195</v>
@@ -10365,11 +10366,11 @@
         <v>3</v>
       </c>
       <c r="K40" s="7"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
       <c r="N40" s="7"/>
       <c r="O40" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -10389,10 +10390,10 @@
         <v>198</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F41" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>186</v>
@@ -10411,7 +10412,7 @@
       <c r="M41" s="7"/>
       <c r="N41" s="7"/>
       <c r="O41" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
@@ -10431,10 +10432,10 @@
         <v>198</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F42" s="21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>186</v>
@@ -10453,7 +10454,7 @@
       <c r="M42" s="7"/>
       <c r="N42" s="7"/>
       <c r="O42" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
@@ -10473,10 +10474,10 @@
         <v>198</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F43" s="21">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>186</v>
@@ -10495,7 +10496,7 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
@@ -10515,10 +10516,10 @@
         <v>198</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F44" s="21">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>186</v>
@@ -10537,7 +10538,7 @@
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
       <c r="O44" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -10557,22 +10558,20 @@
         <v>198</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F45" s="21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>186</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="I45" s="12" t="s">
-        <v>196</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="I45" s="12"/>
       <c r="J45" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
@@ -10599,10 +10598,10 @@
         <v>198</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F46" s="21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>186</v>
@@ -10619,7 +10618,7 @@
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
       <c r="O46" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P46" s="7"/>
       <c r="Q46" s="7"/>
@@ -10639,13 +10638,13 @@
         <v>198</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F47" s="21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>197</v>
@@ -10659,7 +10658,7 @@
       <c r="M47" s="7"/>
       <c r="N47" s="7"/>
       <c r="O47" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P47" s="7"/>
       <c r="Q47" s="7"/>
@@ -10678,14 +10677,14 @@
       <c r="D48" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>114</v>
+      <c r="E48" s="62" t="s">
+        <v>117</v>
       </c>
       <c r="F48" s="21">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G48" s="12" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H48" s="12" t="s">
         <v>197</v>
@@ -10699,7 +10698,7 @@
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
       <c r="O48" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P48" s="7"/>
       <c r="Q48" s="7"/>
@@ -10718,11 +10717,11 @@
       <c r="D49" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="E49" s="62" t="s">
-        <v>117</v>
+      <c r="E49" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="F49" s="21">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>186</v>
@@ -10739,7 +10738,7 @@
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
       <c r="O49" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
@@ -10759,10 +10758,10 @@
         <v>198</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F50" s="21">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>186</v>
@@ -10770,7 +10769,7 @@
       <c r="H50" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="I50" s="12"/>
+      <c r="I50" s="7"/>
       <c r="J50" s="21">
         <v>4</v>
       </c>
@@ -10779,7 +10778,7 @@
       <c r="M50" s="7"/>
       <c r="N50" s="7"/>
       <c r="O50" s="12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="P50" s="7"/>
       <c r="Q50" s="7"/>
@@ -10799,10 +10798,10 @@
         <v>198</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F51" s="21">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>186</v>
@@ -10810,7 +10809,7 @@
       <c r="H51" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="I51" s="7"/>
+      <c r="I51" s="12"/>
       <c r="J51" s="21">
         <v>4</v>
       </c>
@@ -10819,7 +10818,7 @@
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
       <c r="O51" s="12" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="P51" s="7"/>
       <c r="Q51" s="7"/>
@@ -10835,22 +10834,24 @@
       <c r="C52" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>123</v>
+      <c r="D52" s="63" t="s">
+        <v>354</v>
+      </c>
+      <c r="E52" s="62" t="s">
+        <v>373</v>
       </c>
       <c r="F52" s="21">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="H52" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="H52" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="I52" s="12"/>
+      <c r="I52" s="62" t="s">
+        <v>371</v>
+      </c>
       <c r="J52" s="21">
         <v>4</v>
       </c>
@@ -10858,8 +10859,8 @@
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
-      <c r="O52" s="12" t="s">
-        <v>191</v>
+      <c r="O52" s="62" t="s">
+        <v>189</v>
       </c>
       <c r="P52" s="7"/>
       <c r="Q52" s="7"/>
@@ -10875,32 +10876,32 @@
       <c r="C53" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="D53" s="63" t="s">
-        <v>354</v>
-      </c>
-      <c r="E53" s="62" t="s">
-        <v>373</v>
+      <c r="D53" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="F53" s="21">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>370</v>
-      </c>
-      <c r="H53" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="I53" s="62" t="s">
-        <v>371</v>
+        <v>186</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="J53" s="21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="62" t="s">
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12" t="s">
         <v>189</v>
       </c>
       <c r="P53" s="7"/>
@@ -10908,6 +10909,7 @@
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
       <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
     </row>
     <row r="54" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
@@ -10921,22 +10923,22 @@
         <v>375</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>80</v>
+        <v>377</v>
       </c>
       <c r="F54" s="21">
         <v>9</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>188</v>
+        <v>379</v>
       </c>
       <c r="J54" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K54" s="7"/>
       <c r="L54" s="12"/>
@@ -10950,53 +10952,10 @@
       <c r="R54" s="7"/>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
-      <c r="U54" s="7"/>
-    </row>
-    <row r="55" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11">
-        <v>44075</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>375</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="F55" s="21">
-        <v>9</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="I55" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="J55" s="21">
-        <v>2</v>
-      </c>
-      <c r="K55" s="7"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="71"/>
-    </row>
-    <row r="57" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="72"/>
+      <c r="U54" s="71"/>
+    </row>
+    <row r="56" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.51180599999999998"/>

</xml_diff>